<commit_message>
Model Spawn Added. Marker spawn Added.
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -35,13 +35,13 @@
     <t xml:space="preserve">test_files_path</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/stb21753492/FiducialTags/</t>
+    <t xml:space="preserve">/home/stb21753492/FiducialTags/Simulations</t>
   </si>
   <si>
     <t xml:space="preserve">world_file</t>
   </si>
   <si>
-    <t xml:space="preserve">1_marker_small.sdf</t>
+    <t xml:space="preserve">standard_world.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">movement_path</t>
@@ -77,13 +77,13 @@
     <t xml:space="preserve">models</t>
   </si>
   <si>
-    <t xml:space="preserve">model1.sdf</t>
+    <t xml:space="preserve">DICT_4X4_50_s500_id0.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">0,0,1,0,1,0</t>
   </si>
   <si>
-    <t xml:space="preserve">model2.sdf</t>
+    <t xml:space="preserve">DICT_4X4_50_s500_id1.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">0,0,0,0,0,0</t>
@@ -104,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -192,13 +193,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.87"/>
   </cols>
   <sheetData>
@@ -248,10 +249,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>

</xml_diff>

<commit_message>
Marker and Camera Load updated. Variable name vs file difference updated
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">pose_test.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">video_name</t>
+    <t xml:space="preserve">video_file</t>
   </si>
   <si>
     <t xml:space="preserve">video.mp4</t>
@@ -68,25 +68,25 @@
     <t xml:space="preserve">cameras</t>
   </si>
   <si>
-    <t xml:space="preserve">camera1.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,0,0,1,1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">models</t>
+    <t xml:space="preserve">Cam_Basic.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">markers</t>
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id0.sdf</t>
   </si>
   <si>
-    <t xml:space="preserve">0,0,1,0,1,0</t>
+    <t xml:space="preserve">1,1,0.5,0.72,0,0</t>
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id1.sdf</t>
   </si>
   <si>
-    <t xml:space="preserve">0,0,0,0,0,0</t>
+    <t xml:space="preserve">-1,0,0.1,0,0.52,0</t>
   </si>
   <si>
     <t xml:space="preserve">lights</t>
@@ -193,7 +193,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,7 +249,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Video Start/Stop Record Added
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">standard_world.sdf</t>
   </si>
   <si>
-    <t xml:space="preserve">movement_path</t>
+    <t xml:space="preserve">movement_file</t>
   </si>
   <si>
     <t xml:space="preserve">pose_test.txt</t>
@@ -68,7 +68,7 @@
     <t xml:space="preserve">cameras</t>
   </si>
   <si>
-    <t xml:space="preserve">Cam_Basic.sdf</t>
+    <t xml:space="preserve">Cam_Basic_no_topic.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">1,1,1,0,0,0</t>
@@ -196,7 +196,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -249,10 +249,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>

</xml_diff>

<commit_message>
Wait until movement complete Added
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Tested" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -53,13 +54,7 @@
     <t xml:space="preserve">video_file</t>
   </si>
   <si>
-    <t xml:space="preserve">video.mp4</t>
-  </si>
-  <si>
     <t xml:space="preserve">gz_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gzpose.txt</t>
   </si>
   <si>
     <t xml:space="preserve">vid_pose_file</t>
@@ -196,7 +191,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -248,11 +243,11 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -282,56 +277,59 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -343,4 +341,111 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Camera Config file added
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">cameras</t>
   </si>
   <si>
-    <t xml:space="preserve">Cam_Basic_no_topic.sdf</t>
+    <t xml:space="preserve">Cam_Stereo.sdf</t>
   </si>
   <si>
     <t xml:space="preserve">1,1,1,0,0,0</t>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1,0.5,0.72,0,0</t>
   </si>
   <si>
     <t xml:space="preserve">DICT_4X4_50_s500_id1.sdf</t>
@@ -190,7 +187,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -243,10 +240,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -314,21 +311,21 @@
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
+      <c r="C7" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stereo record implemented from Camera config
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -187,7 +187,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -240,10 +240,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -274,7 +274,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,7 +290,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Tests Updated (Rotation test added)
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -9,9 +9,10 @@
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Test_1a" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Test_1b" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Test_1c" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Test_1_rotation" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Test_1a" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Test_1b" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Test_1c" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -49,43 +50,46 @@
     <t xml:space="preserve">movement_file</t>
   </si>
   <si>
+    <t xml:space="preserve">rotate.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gz_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vid_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cameras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KahnPhone.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">markers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,-1,0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">models</t>
+  </si>
+  <si>
     <t xml:space="preserve">pose_test.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">video_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gz_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vid_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cameras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KahnPhone.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1,1,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">markers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,-1,0,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">models</t>
   </si>
   <si>
     <t xml:space="preserve">pose_test_2.txt</t>
@@ -204,10 +208,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B7:B8 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -260,10 +264,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B8"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -369,10 +373,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7:B8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -446,7 +450,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,10 +482,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B7:B8 B6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -504,7 +508,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,15 +551,124 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Mult new tests added (for pose extraction verification)
</commit_message>
<xml_diff>
--- a/Simulations/Test.xlsx
+++ b/Simulations/Test.xlsx
@@ -9,10 +9,13 @@
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Test_1_rotation" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Test_1a" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Test_1b" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Test_1c" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="roll_and_pitch_new" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Lin_New" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Rotation_new" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Test_1_rotation" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Test_1a" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Test_1b" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Test_1c" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="31">
   <si>
     <t xml:space="preserve">Parameter</t>
   </si>
@@ -50,43 +53,55 @@
     <t xml:space="preserve">movement_file</t>
   </si>
   <si>
+    <t xml:space="preserve">roll_and_pitch_new.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">video_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gz_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vid_pose_file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cameras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KahnPhone_new.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1,1,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">markers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1,-1,0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lin_move_new.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate_new.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">rotate.txt</t>
   </si>
   <si>
-    <t xml:space="preserve">video_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gz_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vid_pose_file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cameras</t>
-  </si>
-  <si>
     <t xml:space="preserve">KahnPhone.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,1,1,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">markers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s100_id0.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DICT_4X4_50_s100_id1.sdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1,-1,0,0,0,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lights</t>
-  </si>
-  <si>
-    <t xml:space="preserve">models</t>
   </si>
   <si>
     <t xml:space="preserve">pose_test.txt</t>
@@ -211,7 +226,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -267,7 +282,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -373,10 +388,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -482,10 +497,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -559,7 +574,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,10 +606,10 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
@@ -617,7 +632,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +664,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -660,15 +675,342 @@
         <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.03"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>